<commit_message>
Working on Invoice Lines writing
</commit_message>
<xml_diff>
--- a/06-python/src/comp230-excel/comp_230.xlsx
+++ b/06-python/src/comp230-excel/comp_230.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\urank\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E997CF53-FBAB-4E2A-B638-0094A24D485B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A30730-D93D-4210-92BC-579674B3A7B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="821" activeTab="2" xr2:uid="{372980B3-46BC-4154-BAD1-391F1841EC37}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
     <sheet name="Invoices" sheetId="5" r:id="rId2"/>
-    <sheet name="Line Items" sheetId="7" r:id="rId3"/>
+    <sheet name="Line Items" sheetId="8" r:id="rId3"/>
     <sheet name="Products" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -852,7 +852,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -879,6 +879,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2029,10 +2033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC0F608-E94A-4DBC-8A6D-99BBE8FE3CC6}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,7 +2044,7 @@
     <col min="1" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -2057,7 +2061,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2070,11 +2074,12 @@
       <c r="D2" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E2" s="9">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="11">
+        <v>294.5</v>
+      </c>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2087,11 +2092,11 @@
       <c r="D3" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="11">
         <v>1282.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2108,7 +2113,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2125,7 +2130,7 @@
         <v>464.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2142,7 +2147,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2155,11 +2160,11 @@
       <c r="D7" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E7" s="9">
-        <v>1303.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="11">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2176,7 +2181,7 @@
         <v>150.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2193,7 +2198,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2216,7 +2221,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461ADDC3-2EB0-4A9A-AC6B-12E71E4208D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB34AAB9-723F-4595-B57A-DEB7BB8C5B6D}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2224,9 +2229,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="5" width="15.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
Completed Comp230 part 1
</commit_message>
<xml_diff>
--- a/06-python/src/comp230-excel/comp_230.xlsx
+++ b/06-python/src/comp230-excel/comp_230.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\urank\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\cohort4\06-python\src\comp230-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A30730-D93D-4210-92BC-579674B3A7B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783600AD-AD60-424D-8B3C-C36794B3A526}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="821" activeTab="2" xr2:uid="{372980B3-46BC-4154-BAD1-391F1841EC37}"/>
+    <workbookView xWindow="150" yWindow="90" windowWidth="9450" windowHeight="15255" tabRatio="821" activeTab="1" xr2:uid="{372980B3-46BC-4154-BAD1-391F1841EC37}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -2035,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC0F608-E94A-4DBC-8A6D-99BBE8FE3CC6}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,7 +2161,7 @@
         <v>197</v>
       </c>
       <c r="E7" s="11">
-        <v>1686</v>
+        <v>1303.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2224,11 +2224,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB34AAB9-723F-4595-B57A-DEB7BB8C5B6D}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -2499,7 +2502,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="7">
-        <v>425</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>